<commit_message>
change the payment method to Amex Ezeclick in Excel
</commit_message>
<xml_diff>
--- a/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
+++ b/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Airpay_Updated\Airpay_Automation_Framework\AirPayTestData\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shishir.shah\AirpayAutomationProject_Updated\Airpay_Automation_Framework\AirPayTestData\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BCC7D5-BA5B-4490-9C07-836384995B1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NoramlKit" sheetId="1" r:id="rId1"/>
@@ -2345,13 +2346,13 @@
     <t>With surcharge amount check(This channel moved into Virtual Account, so no need to run these cases</t>
   </si>
   <si>
-    <t>IE</t>
+    <t>http://localhost/airpay_php_live/transaction.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3120,15 +3121,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BY302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3449,7 +3450,7 @@
         <v>701</v>
       </c>
       <c r="D3" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3501,7 +3502,7 @@
         <v>701</v>
       </c>
       <c r="D4" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3549,7 +3550,7 @@
         <v>701</v>
       </c>
       <c r="D5" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -3597,7 +3598,7 @@
         <v>701</v>
       </c>
       <c r="D6" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3648,7 +3649,7 @@
         <v>701</v>
       </c>
       <c r="D7" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3693,7 +3694,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3734,7 +3735,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -3779,7 +3780,7 @@
         <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -3824,7 +3825,7 @@
         <v>701</v>
       </c>
       <c r="D11" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3884,7 +3885,7 @@
         <v>701</v>
       </c>
       <c r="D12" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -3944,7 +3945,7 @@
         <v>701</v>
       </c>
       <c r="D13" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -4004,7 +4005,7 @@
         <v>701</v>
       </c>
       <c r="D14" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -4049,7 +4050,7 @@
         <v>701</v>
       </c>
       <c r="D15" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -4109,7 +4110,7 @@
         <v>701</v>
       </c>
       <c r="D16" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -4169,7 +4170,7 @@
         <v>701</v>
       </c>
       <c r="D17" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -4229,7 +4230,7 @@
         <v>701</v>
       </c>
       <c r="D18" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4289,7 +4290,7 @@
         <v>701</v>
       </c>
       <c r="D19" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -4349,7 +4350,7 @@
         <v>22</v>
       </c>
       <c r="D20" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -4407,7 +4408,7 @@
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -4465,7 +4466,7 @@
         <v>22</v>
       </c>
       <c r="D22" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -4523,7 +4524,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -4580,7 +4581,7 @@
         <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -4637,7 +4638,7 @@
         <v>701</v>
       </c>
       <c r="D25" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -4684,7 +4685,7 @@
         <v>701</v>
       </c>
       <c r="D26" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -4693,7 +4694,7 @@
         <v>506</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>24</v>
@@ -4720,7 +4721,7 @@
         <v>35</v>
       </c>
       <c r="AB26" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF26" s="5"/>
       <c r="AG26" s="5"/>
@@ -4737,7 +4738,7 @@
         <v>701</v>
       </c>
       <c r="D27" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -4746,7 +4747,7 @@
         <v>84</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>24</v>
@@ -4773,7 +4774,7 @@
         <v>35</v>
       </c>
       <c r="AB27" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF27" s="5"/>
       <c r="AG27" s="5"/>
@@ -4791,7 +4792,7 @@
         <v>701</v>
       </c>
       <c r="D28" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -4835,7 +4836,7 @@
         <v>701</v>
       </c>
       <c r="D29" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -4879,7 +4880,7 @@
         <v>701</v>
       </c>
       <c r="D30" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -4924,7 +4925,7 @@
         <v>701</v>
       </c>
       <c r="D31" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -4968,7 +4969,7 @@
         <v>701</v>
       </c>
       <c r="D32" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -5015,7 +5016,7 @@
         <v>701</v>
       </c>
       <c r="D33" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -5062,7 +5063,7 @@
         <v>701</v>
       </c>
       <c r="D34" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -5109,7 +5110,7 @@
         <v>701</v>
       </c>
       <c r="D35" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -5166,7 +5167,7 @@
         <v>22</v>
       </c>
       <c r="D36" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -5221,7 +5222,7 @@
         <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -5276,7 +5277,7 @@
         <v>22</v>
       </c>
       <c r="D38" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -5331,7 +5332,7 @@
         <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -5386,7 +5387,7 @@
         <v>22</v>
       </c>
       <c r="D40" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -5441,7 +5442,7 @@
         <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -5495,7 +5496,7 @@
         <v>22</v>
       </c>
       <c r="D42" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -5549,7 +5550,7 @@
         <v>22</v>
       </c>
       <c r="D43" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -5603,7 +5604,7 @@
         <v>22</v>
       </c>
       <c r="D44" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -5657,7 +5658,7 @@
         <v>22</v>
       </c>
       <c r="D45" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -5711,7 +5712,7 @@
         <v>701</v>
       </c>
       <c r="D46" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -5755,7 +5756,7 @@
         <v>701</v>
       </c>
       <c r="D47" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -5764,7 +5765,7 @@
         <v>126</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>24</v>
@@ -5788,7 +5789,7 @@
         <v>125</v>
       </c>
       <c r="AB47" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF47" s="5"/>
       <c r="AG47" s="5"/>
@@ -5805,7 +5806,7 @@
         <v>701</v>
       </c>
       <c r="D48" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -5849,7 +5850,7 @@
         <v>701</v>
       </c>
       <c r="D49" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -5893,7 +5894,7 @@
         <v>701</v>
       </c>
       <c r="D50" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -5937,7 +5938,7 @@
         <v>701</v>
       </c>
       <c r="D51" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -5981,7 +5982,7 @@
         <v>701</v>
       </c>
       <c r="D52" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -6025,7 +6026,7 @@
         <v>701</v>
       </c>
       <c r="D53" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -6034,7 +6035,7 @@
         <v>142</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>24</v>
@@ -6061,7 +6062,7 @@
         <v>125</v>
       </c>
       <c r="AB53" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF53" s="5"/>
       <c r="AG53" s="5"/>
@@ -6078,7 +6079,7 @@
         <v>701</v>
       </c>
       <c r="D54" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -6120,7 +6121,7 @@
         <v>149</v>
       </c>
       <c r="AB54" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
     </row>
     <row r="55" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -6134,7 +6135,7 @@
         <v>701</v>
       </c>
       <c r="D55" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E55">
         <v>1</v>
@@ -6187,7 +6188,7 @@
         <v>701</v>
       </c>
       <c r="D56" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -6240,7 +6241,7 @@
         <v>701</v>
       </c>
       <c r="D57" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -6293,7 +6294,7 @@
         <v>701</v>
       </c>
       <c r="D58" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -6346,7 +6347,7 @@
         <v>701</v>
       </c>
       <c r="D59" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -6399,7 +6400,7 @@
         <v>701</v>
       </c>
       <c r="D60" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -6452,7 +6453,7 @@
         <v>701</v>
       </c>
       <c r="D61" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -6505,7 +6506,7 @@
         <v>22</v>
       </c>
       <c r="D62" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -6547,7 +6548,7 @@
         <v>22</v>
       </c>
       <c r="D63" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -6589,7 +6590,7 @@
         <v>22</v>
       </c>
       <c r="D64" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -6631,7 +6632,7 @@
         <v>22</v>
       </c>
       <c r="D65" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -6673,7 +6674,7 @@
         <v>22</v>
       </c>
       <c r="D66" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -6715,7 +6716,7 @@
         <v>22</v>
       </c>
       <c r="D67" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -6749,7 +6750,7 @@
     <row r="68" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="34"/>
       <c r="D68" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
@@ -6768,7 +6769,7 @@
         <v>22</v>
       </c>
       <c r="D69" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -6830,7 +6831,7 @@
         <v>22</v>
       </c>
       <c r="D70" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -6892,7 +6893,7 @@
         <v>22</v>
       </c>
       <c r="D71" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -6954,7 +6955,7 @@
         <v>22</v>
       </c>
       <c r="D72" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -7016,7 +7017,7 @@
         <v>22</v>
       </c>
       <c r="D73" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -7071,7 +7072,7 @@
       <c r="A74" s="34"/>
       <c r="C74" s="15"/>
       <c r="D74" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
@@ -7090,7 +7091,7 @@
         <v>701</v>
       </c>
       <c r="D75" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -7134,7 +7135,7 @@
         <v>701</v>
       </c>
       <c r="D76" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -7187,7 +7188,7 @@
         <v>701</v>
       </c>
       <c r="D77" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -7240,7 +7241,7 @@
         <v>701</v>
       </c>
       <c r="D78" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -7289,7 +7290,7 @@
         <v>701</v>
       </c>
       <c r="D79" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -7333,7 +7334,7 @@
         <v>701</v>
       </c>
       <c r="D80" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -7374,7 +7375,7 @@
         <v>701</v>
       </c>
       <c r="D81" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -7415,7 +7416,7 @@
         <v>701</v>
       </c>
       <c r="D82" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -7456,7 +7457,7 @@
         <v>701</v>
       </c>
       <c r="D83" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -7483,7 +7484,7 @@
         <v>33</v>
       </c>
       <c r="O83" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:38" ht="15" x14ac:dyDescent="0.25">
@@ -7497,7 +7498,7 @@
         <v>701</v>
       </c>
       <c r="D84" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -7538,7 +7539,7 @@
         <v>701</v>
       </c>
       <c r="D85" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -7592,7 +7593,7 @@
         <v>22</v>
       </c>
       <c r="D86" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -7646,7 +7647,7 @@
         <v>22</v>
       </c>
       <c r="D87" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -7700,7 +7701,7 @@
         <v>22</v>
       </c>
       <c r="D88" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -7754,7 +7755,7 @@
         <v>22</v>
       </c>
       <c r="D89" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -7808,7 +7809,7 @@
         <v>22</v>
       </c>
       <c r="D90" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -7862,7 +7863,7 @@
         <v>22</v>
       </c>
       <c r="D91" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -7916,7 +7917,7 @@
         <v>22</v>
       </c>
       <c r="D92" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E92">
         <v>1</v>
@@ -7931,7 +7932,7 @@
     <row r="93" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A93" s="34"/>
       <c r="D93" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
     </row>
     <row r="94" spans="1:38" ht="15" x14ac:dyDescent="0.25">
@@ -7945,7 +7946,7 @@
         <v>22</v>
       </c>
       <c r="D94" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -7997,7 +7998,7 @@
         <v>22</v>
       </c>
       <c r="D95" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -8049,7 +8050,7 @@
         <v>22</v>
       </c>
       <c r="D96" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -8101,7 +8102,7 @@
         <v>22</v>
       </c>
       <c r="D97" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -8137,7 +8138,7 @@
     <row r="98" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A98" s="34"/>
       <c r="D98" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
     </row>
     <row r="99" spans="1:77" ht="15" x14ac:dyDescent="0.25">
@@ -8151,7 +8152,7 @@
         <v>22</v>
       </c>
       <c r="D99" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -8163,7 +8164,7 @@
         <v>768</v>
       </c>
       <c r="AB99" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF99" t="s">
         <v>227</v>
@@ -8189,7 +8190,7 @@
         <v>22</v>
       </c>
       <c r="D100" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E100">
         <v>1</v>
@@ -8219,7 +8220,7 @@
         <v>46</v>
       </c>
       <c r="AB100" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF100" t="s">
         <v>227</v>
@@ -8245,7 +8246,7 @@
         <v>22</v>
       </c>
       <c r="D101" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -8275,7 +8276,7 @@
         <v>46</v>
       </c>
       <c r="AB101" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF101" t="s">
         <v>227</v>
@@ -8301,7 +8302,7 @@
         <v>22</v>
       </c>
       <c r="D102" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E102">
         <v>1</v>
@@ -8331,7 +8332,7 @@
         <v>54</v>
       </c>
       <c r="AB102" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF102" t="s">
         <v>227</v>
@@ -8357,7 +8358,7 @@
         <v>22</v>
       </c>
       <c r="D103" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E103">
         <v>1</v>
@@ -8387,7 +8388,7 @@
         <v>54</v>
       </c>
       <c r="AB103" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF103" t="s">
         <v>227</v>
@@ -8413,7 +8414,7 @@
         <v>22</v>
       </c>
       <c r="D104" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E104">
         <v>1</v>
@@ -8443,7 +8444,7 @@
         <v>46</v>
       </c>
       <c r="AB104" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF104" t="s">
         <v>227</v>
@@ -8469,7 +8470,7 @@
         <v>22</v>
       </c>
       <c r="D105" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -8499,7 +8500,7 @@
         <v>46</v>
       </c>
       <c r="AB105" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF105" t="s">
         <v>227</v>
@@ -8525,7 +8526,7 @@
         <v>22</v>
       </c>
       <c r="D106" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -8555,7 +8556,7 @@
         <v>54</v>
       </c>
       <c r="AB106" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF106" t="s">
         <v>227</v>
@@ -8581,7 +8582,7 @@
         <v>22</v>
       </c>
       <c r="D107" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E107">
         <v>1</v>
@@ -8611,7 +8612,7 @@
         <v>54</v>
       </c>
       <c r="AB107" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF107" t="s">
         <v>227</v>
@@ -8637,7 +8638,7 @@
         <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E108" s="25">
         <v>1</v>
@@ -8689,7 +8690,7 @@
       <c r="Z108" s="25"/>
       <c r="AA108" s="25"/>
       <c r="AB108" s="25" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC108" s="25"/>
       <c r="AD108" s="25"/>
@@ -8769,7 +8770,7 @@
         <v>22</v>
       </c>
       <c r="D109" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -8814,7 +8815,7 @@
       <c r="W109" s="25"/>
       <c r="X109" s="25"/>
       <c r="AB109" s="25" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC109" s="25"/>
       <c r="AD109" s="25"/>
@@ -8852,7 +8853,7 @@
     </row>
     <row r="110" spans="1:77" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:77" ht="15" x14ac:dyDescent="0.25">
@@ -8866,7 +8867,7 @@
         <v>22</v>
       </c>
       <c r="D111" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -8900,7 +8901,7 @@
         <v>77</v>
       </c>
       <c r="AB111" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC111" s="21"/>
       <c r="AD111" s="21"/>
@@ -8950,7 +8951,7 @@
         <v>22</v>
       </c>
       <c r="D112" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -8984,7 +8985,7 @@
         <v>77</v>
       </c>
       <c r="AB112" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC112" s="21"/>
       <c r="AD112" s="21"/>
@@ -9034,7 +9035,7 @@
         <v>22</v>
       </c>
       <c r="D113" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -9068,7 +9069,7 @@
         <v>77</v>
       </c>
       <c r="AB113" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC113" s="21"/>
       <c r="AD113" s="21"/>
@@ -9118,7 +9119,7 @@
         <v>22</v>
       </c>
       <c r="D114" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E114">
         <v>1</v>
@@ -9152,7 +9153,7 @@
         <v>77</v>
       </c>
       <c r="AB114" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC114" s="21"/>
       <c r="AD114" s="21"/>
@@ -9202,7 +9203,7 @@
         <v>22</v>
       </c>
       <c r="D115" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E115">
         <v>1</v>
@@ -9236,7 +9237,7 @@
         <v>77</v>
       </c>
       <c r="AB115" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC115" s="21"/>
       <c r="AD115" s="21"/>
@@ -9292,7 +9293,7 @@
         <v>22</v>
       </c>
       <c r="D116" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E116">
         <v>1</v>
@@ -9326,7 +9327,7 @@
         <v>77</v>
       </c>
       <c r="AB116" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC116" s="21"/>
       <c r="AD116" s="21"/>
@@ -9373,7 +9374,7 @@
     </row>
     <row r="117" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H117" s="23"/>
       <c r="I117" s="1"/>
@@ -9411,7 +9412,7 @@
         <v>22</v>
       </c>
       <c r="D118" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E118">
         <v>1</v>
@@ -9442,7 +9443,7 @@
         <v>87</v>
       </c>
       <c r="AB118" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC118" s="21"/>
       <c r="AD118" s="21"/>
@@ -9492,7 +9493,7 @@
         <v>22</v>
       </c>
       <c r="D119" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E119">
         <v>1</v>
@@ -9523,7 +9524,7 @@
         <v>87</v>
       </c>
       <c r="AB119" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC119" s="21"/>
       <c r="AD119" s="21"/>
@@ -9573,7 +9574,7 @@
         <v>22</v>
       </c>
       <c r="D120" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E120">
         <v>1</v>
@@ -9604,7 +9605,7 @@
         <v>87</v>
       </c>
       <c r="AB120" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC120" s="21"/>
       <c r="AD120" s="21"/>
@@ -9654,7 +9655,7 @@
         <v>22</v>
       </c>
       <c r="D121" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E121">
         <v>1</v>
@@ -9685,7 +9686,7 @@
         <v>87</v>
       </c>
       <c r="AB121" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC121" s="21"/>
       <c r="AD121" s="21"/>
@@ -9735,7 +9736,7 @@
         <v>22</v>
       </c>
       <c r="D122" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E122">
         <v>1</v>
@@ -9769,7 +9770,7 @@
         <v>87</v>
       </c>
       <c r="AB122" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC122" s="21"/>
       <c r="AD122" s="21"/>
@@ -9825,7 +9826,7 @@
         <v>22</v>
       </c>
       <c r="D123" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E123">
         <v>1</v>
@@ -9859,7 +9860,7 @@
         <v>87</v>
       </c>
       <c r="AB123" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC123" s="21"/>
       <c r="AD123" s="21"/>
@@ -9915,7 +9916,7 @@
         <v>22</v>
       </c>
       <c r="D124" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E124">
         <v>1</v>
@@ -9952,7 +9953,7 @@
         <v>87</v>
       </c>
       <c r="AB124" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC124" s="21"/>
       <c r="AD124" s="21"/>
@@ -9999,7 +10000,7 @@
     </row>
     <row r="125" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E125">
         <v>1</v>
@@ -10017,7 +10018,7 @@
         <v>22</v>
       </c>
       <c r="D126" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E126">
         <v>1</v>
@@ -10051,7 +10052,7 @@
         <v>293</v>
       </c>
       <c r="AB126" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC126" s="21"/>
       <c r="AD126" s="21"/>
@@ -10101,7 +10102,7 @@
         <v>22</v>
       </c>
       <c r="D127" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E127">
         <v>1</v>
@@ -10135,7 +10136,7 @@
         <v>293</v>
       </c>
       <c r="AB127" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC127" s="21"/>
       <c r="AD127" s="21"/>
@@ -10185,7 +10186,7 @@
         <v>22</v>
       </c>
       <c r="D128" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E128">
         <v>1</v>
@@ -10219,7 +10220,7 @@
         <v>293</v>
       </c>
       <c r="AB128" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC128" s="21"/>
       <c r="AD128" s="21"/>
@@ -10269,7 +10270,7 @@
         <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E129">
         <v>1</v>
@@ -10303,7 +10304,7 @@
         <v>293</v>
       </c>
       <c r="AB129" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC129" s="21"/>
       <c r="AD129" s="21"/>
@@ -10353,7 +10354,7 @@
         <v>22</v>
       </c>
       <c r="D130" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E130">
         <v>1</v>
@@ -10387,7 +10388,7 @@
         <v>293</v>
       </c>
       <c r="AB130" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC130" s="21"/>
       <c r="AD130" s="21"/>
@@ -10443,7 +10444,7 @@
         <v>22</v>
       </c>
       <c r="D131" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -10477,7 +10478,7 @@
         <v>293</v>
       </c>
       <c r="AB131" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC131" s="21"/>
       <c r="AD131" s="21"/>
@@ -10533,7 +10534,7 @@
         <v>22</v>
       </c>
       <c r="D132" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E132">
         <v>1</v>
@@ -10570,7 +10571,7 @@
         <v>431</v>
       </c>
       <c r="AB132" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC132" s="21"/>
       <c r="AD132" s="21"/>
@@ -10617,7 +10618,7 @@
     </row>
     <row r="133" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -10635,7 +10636,7 @@
         <v>22</v>
       </c>
       <c r="D134" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E134">
         <v>1</v>
@@ -10672,7 +10673,7 @@
         <v>302</v>
       </c>
       <c r="AB134" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC134" s="21"/>
       <c r="AD134" s="21"/>
@@ -10722,7 +10723,7 @@
         <v>22</v>
       </c>
       <c r="D135" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E135">
         <v>1</v>
@@ -10759,7 +10760,7 @@
         <v>302</v>
       </c>
       <c r="AB135" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC135" s="21"/>
       <c r="AD135" s="21"/>
@@ -10809,7 +10810,7 @@
         <v>22</v>
       </c>
       <c r="D136" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E136">
         <v>1</v>
@@ -10843,7 +10844,7 @@
         <v>168</v>
       </c>
       <c r="AB136" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC136" s="21"/>
       <c r="AD136" s="21"/>
@@ -10893,7 +10894,7 @@
         <v>22</v>
       </c>
       <c r="D137" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E137">
         <v>1</v>
@@ -10927,7 +10928,7 @@
         <v>168</v>
       </c>
       <c r="AB137" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC137" s="21"/>
       <c r="AD137" s="21"/>
@@ -10977,7 +10978,7 @@
         <v>22</v>
       </c>
       <c r="D138" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E138">
         <v>1</v>
@@ -11011,7 +11012,7 @@
         <v>168</v>
       </c>
       <c r="AB138" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC138" s="21"/>
       <c r="AD138" s="21"/>
@@ -11067,7 +11068,7 @@
         <v>22</v>
       </c>
       <c r="D139" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E139">
         <v>1</v>
@@ -11101,7 +11102,7 @@
         <v>168</v>
       </c>
       <c r="AB139" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC139" s="21"/>
       <c r="AD139" s="21"/>
@@ -11151,7 +11152,7 @@
         <v>309</v>
       </c>
       <c r="D140" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E140">
         <v>1</v>
@@ -11160,7 +11161,7 @@
     </row>
     <row r="141" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E141">
         <v>1</v>
@@ -11178,7 +11179,7 @@
         <v>22</v>
       </c>
       <c r="D142" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E142">
         <v>1</v>
@@ -11215,7 +11216,7 @@
         <v>302</v>
       </c>
       <c r="AB142" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC142" s="21"/>
       <c r="AD142" s="21"/>
@@ -11265,7 +11266,7 @@
         <v>22</v>
       </c>
       <c r="D143" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E143">
         <v>1</v>
@@ -11302,7 +11303,7 @@
         <v>302</v>
       </c>
       <c r="AB143" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC143" s="21"/>
       <c r="AD143" s="21"/>
@@ -11352,7 +11353,7 @@
         <v>22</v>
       </c>
       <c r="D144" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E144">
         <v>1</v>
@@ -11386,7 +11387,7 @@
         <v>312</v>
       </c>
       <c r="AB144" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC144" s="21"/>
       <c r="AD144" s="21"/>
@@ -11436,7 +11437,7 @@
         <v>22</v>
       </c>
       <c r="D145" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E145">
         <v>1</v>
@@ -11470,7 +11471,7 @@
         <v>312</v>
       </c>
       <c r="AB145" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC145" s="21"/>
       <c r="AD145" s="21"/>
@@ -11520,7 +11521,7 @@
         <v>22</v>
       </c>
       <c r="D146" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E146">
         <v>1</v>
@@ -11554,7 +11555,7 @@
         <v>312</v>
       </c>
       <c r="AB146" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC146" s="21"/>
       <c r="AD146" s="21"/>
@@ -11610,7 +11611,7 @@
         <v>22</v>
       </c>
       <c r="D147" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E147">
         <v>1</v>
@@ -11644,7 +11645,7 @@
         <v>312</v>
       </c>
       <c r="AB147" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC147" s="21"/>
       <c r="AD147" s="21"/>
@@ -11691,7 +11692,7 @@
     </row>
     <row r="148" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H148" s="23"/>
       <c r="I148" s="1"/>
@@ -11720,7 +11721,7 @@
     </row>
     <row r="149" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E149">
         <v>1</v>
@@ -11738,7 +11739,7 @@
         <v>22</v>
       </c>
       <c r="D150" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E150">
         <v>1</v>
@@ -11775,7 +11776,7 @@
         <v>302</v>
       </c>
       <c r="AB150" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC150" s="21"/>
       <c r="AD150" s="21"/>
@@ -11825,7 +11826,7 @@
         <v>22</v>
       </c>
       <c r="D151" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E151">
         <v>1</v>
@@ -11862,7 +11863,7 @@
         <v>302</v>
       </c>
       <c r="AB151" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC151" s="21"/>
       <c r="AD151" s="21"/>
@@ -11912,7 +11913,7 @@
         <v>22</v>
       </c>
       <c r="D152" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E152">
         <v>1</v>
@@ -11946,7 +11947,7 @@
         <v>326</v>
       </c>
       <c r="AB152" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC152" s="21"/>
       <c r="AD152" s="21"/>
@@ -11996,7 +11997,7 @@
         <v>22</v>
       </c>
       <c r="D153" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E153">
         <v>1</v>
@@ -12030,7 +12031,7 @@
         <v>326</v>
       </c>
       <c r="AB153" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC153" s="21"/>
       <c r="AD153" s="21"/>
@@ -12080,7 +12081,7 @@
         <v>22</v>
       </c>
       <c r="D154" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E154">
         <v>1</v>
@@ -12114,7 +12115,7 @@
         <v>326</v>
       </c>
       <c r="AB154" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC154" s="21"/>
       <c r="AD154" s="21"/>
@@ -12170,7 +12171,7 @@
         <v>22</v>
       </c>
       <c r="D155" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E155">
         <v>1</v>
@@ -12204,7 +12205,7 @@
         <v>326</v>
       </c>
       <c r="AB155" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC155" s="21"/>
       <c r="AD155" s="21"/>
@@ -12260,7 +12261,7 @@
         <v>22</v>
       </c>
       <c r="D156" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E156">
         <v>1</v>
@@ -12294,7 +12295,7 @@
         <v>326</v>
       </c>
       <c r="AB156" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC156" s="21"/>
       <c r="AD156" s="21"/>
@@ -12341,7 +12342,7 @@
     </row>
     <row r="157" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E157">
         <v>1</v>
@@ -12359,7 +12360,7 @@
         <v>22</v>
       </c>
       <c r="D158" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E158">
         <v>1</v>
@@ -12393,7 +12394,7 @@
         <v>208</v>
       </c>
       <c r="AB158" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC158" s="21"/>
       <c r="AD158" s="21"/>
@@ -12443,7 +12444,7 @@
         <v>22</v>
       </c>
       <c r="D159" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E159">
         <v>1</v>
@@ -12480,7 +12481,7 @@
         <v>302</v>
       </c>
       <c r="AB159" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC159" s="21"/>
       <c r="AD159" s="21"/>
@@ -12530,7 +12531,7 @@
         <v>22</v>
       </c>
       <c r="D160" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E160">
         <v>1</v>
@@ -12564,7 +12565,7 @@
         <v>208</v>
       </c>
       <c r="AB160" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC160" s="21"/>
       <c r="AD160" s="21"/>
@@ -12614,7 +12615,7 @@
         <v>22</v>
       </c>
       <c r="D161" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E161">
         <v>1</v>
@@ -12648,7 +12649,7 @@
         <v>208</v>
       </c>
       <c r="AB161" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC161" s="21"/>
       <c r="AD161" s="21"/>
@@ -12698,7 +12699,7 @@
         <v>22</v>
       </c>
       <c r="D162" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E162">
         <v>1</v>
@@ -12732,7 +12733,7 @@
         <v>208</v>
       </c>
       <c r="AB162" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC162" s="21"/>
       <c r="AD162" s="21"/>
@@ -12788,7 +12789,7 @@
         <v>22</v>
       </c>
       <c r="D163" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E163">
         <v>1</v>
@@ -12822,7 +12823,7 @@
         <v>208</v>
       </c>
       <c r="AB163" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC163" s="21"/>
       <c r="AD163" s="21"/>
@@ -12869,7 +12870,7 @@
     </row>
     <row r="164" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H164" s="23"/>
       <c r="I164" s="1"/>
@@ -12900,7 +12901,7 @@
     </row>
     <row r="165" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H165" s="23"/>
       <c r="I165" s="1"/>
@@ -12940,7 +12941,7 @@
         <v>22</v>
       </c>
       <c r="D166" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E166">
         <v>1</v>
@@ -12974,7 +12975,7 @@
         <v>200</v>
       </c>
       <c r="AB166" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC166" s="21"/>
       <c r="AD166" s="21"/>
@@ -13024,7 +13025,7 @@
         <v>22</v>
       </c>
       <c r="D167" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E167">
         <v>1</v>
@@ -13061,7 +13062,7 @@
         <v>302</v>
       </c>
       <c r="AB167" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC167" s="21"/>
       <c r="AD167" s="21"/>
@@ -13111,7 +13112,7 @@
         <v>22</v>
       </c>
       <c r="D168" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E168">
         <v>1</v>
@@ -13145,7 +13146,7 @@
         <v>200</v>
       </c>
       <c r="AB168" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC168" s="21"/>
       <c r="AD168" s="21"/>
@@ -13195,7 +13196,7 @@
         <v>22</v>
       </c>
       <c r="D169" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E169">
         <v>1</v>
@@ -13229,7 +13230,7 @@
         <v>200</v>
       </c>
       <c r="AB169" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC169" s="21"/>
       <c r="AD169" s="21"/>
@@ -13279,7 +13280,7 @@
         <v>22</v>
       </c>
       <c r="D170" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E170">
         <v>1</v>
@@ -13313,7 +13314,7 @@
         <v>200</v>
       </c>
       <c r="AB170" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC170" s="21"/>
       <c r="AD170" s="21"/>
@@ -13369,7 +13370,7 @@
         <v>22</v>
       </c>
       <c r="D171" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E171">
         <v>1</v>
@@ -13403,7 +13404,7 @@
         <v>200</v>
       </c>
       <c r="AB171" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC171" s="21"/>
       <c r="AD171" s="21"/>
@@ -13450,7 +13451,7 @@
     </row>
     <row r="172" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H172" s="23"/>
       <c r="I172" s="1"/>
@@ -13481,7 +13482,7 @@
     </row>
     <row r="173" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H173" s="23"/>
       <c r="I173" s="1"/>
@@ -13521,7 +13522,7 @@
         <v>22</v>
       </c>
       <c r="D174" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E174">
         <v>1</v>
@@ -13555,7 +13556,7 @@
         <v>458</v>
       </c>
       <c r="AB174" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC174" s="21"/>
       <c r="AD174" s="21"/>
@@ -13605,7 +13606,7 @@
         <v>22</v>
       </c>
       <c r="D175" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E175">
         <v>1</v>
@@ -13642,7 +13643,7 @@
         <v>302</v>
       </c>
       <c r="AB175" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC175" s="21"/>
       <c r="AD175" s="21"/>
@@ -13692,7 +13693,7 @@
         <v>22</v>
       </c>
       <c r="D176" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E176">
         <v>1</v>
@@ -13726,7 +13727,7 @@
         <v>458</v>
       </c>
       <c r="AB176" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC176" s="21"/>
       <c r="AD176" s="21"/>
@@ -13776,7 +13777,7 @@
         <v>22</v>
       </c>
       <c r="D177" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E177">
         <v>1</v>
@@ -13810,7 +13811,7 @@
         <v>458</v>
       </c>
       <c r="AB177" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC177" s="21"/>
       <c r="AD177" s="21"/>
@@ -13860,7 +13861,7 @@
         <v>22</v>
       </c>
       <c r="D178" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E178">
         <v>1</v>
@@ -13894,7 +13895,7 @@
         <v>458</v>
       </c>
       <c r="AB178" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC178" s="21"/>
       <c r="AD178" s="21"/>
@@ -13950,7 +13951,7 @@
         <v>22</v>
       </c>
       <c r="D179" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E179">
         <v>1</v>
@@ -13984,7 +13985,7 @@
         <v>458</v>
       </c>
       <c r="AB179" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC179" s="21"/>
       <c r="AD179" s="21"/>
@@ -14031,7 +14032,7 @@
     </row>
     <row r="180" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H180" s="23"/>
       <c r="I180" s="1"/>
@@ -14062,7 +14063,7 @@
     </row>
     <row r="181" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H181" s="23"/>
       <c r="I181" s="1"/>
@@ -14102,7 +14103,7 @@
         <v>22</v>
       </c>
       <c r="D182" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E182">
         <v>1</v>
@@ -14136,7 +14137,7 @@
         <v>205</v>
       </c>
       <c r="AB182" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC182" s="21"/>
       <c r="AD182" s="21"/>
@@ -14180,7 +14181,7 @@
         <v>22</v>
       </c>
       <c r="D183" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E183">
         <v>1</v>
@@ -14217,7 +14218,7 @@
         <v>302</v>
       </c>
       <c r="AB183" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC183" s="21"/>
       <c r="AD183" s="21"/>
@@ -14261,7 +14262,7 @@
         <v>22</v>
       </c>
       <c r="D184" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E184">
         <v>1</v>
@@ -14295,7 +14296,7 @@
         <v>205</v>
       </c>
       <c r="AB184" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC184" s="21"/>
       <c r="AD184" s="21"/>
@@ -14345,7 +14346,7 @@
         <v>22</v>
       </c>
       <c r="D185" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E185">
         <v>1</v>
@@ -14379,7 +14380,7 @@
         <v>205</v>
       </c>
       <c r="AB185" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC185" s="21"/>
       <c r="AD185" s="21"/>
@@ -14429,7 +14430,7 @@
         <v>22</v>
       </c>
       <c r="D186" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E186">
         <v>1</v>
@@ -14463,7 +14464,7 @@
         <v>205</v>
       </c>
       <c r="AB186" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC186" s="21"/>
       <c r="AD186" s="21"/>
@@ -14519,7 +14520,7 @@
         <v>22</v>
       </c>
       <c r="D187" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E187">
         <v>1</v>
@@ -14553,7 +14554,7 @@
         <v>205</v>
       </c>
       <c r="AB187" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC187" s="21"/>
       <c r="AD187" s="21"/>
@@ -14600,7 +14601,7 @@
     </row>
     <row r="188" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H188" s="23"/>
       <c r="I188" s="1"/>
@@ -14640,7 +14641,7 @@
         <v>22</v>
       </c>
       <c r="D189" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E189">
         <v>1</v>
@@ -14674,7 +14675,7 @@
         <v>640</v>
       </c>
       <c r="AB189" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC189" s="21"/>
       <c r="AD189" s="21"/>
@@ -14718,7 +14719,7 @@
         <v>22</v>
       </c>
       <c r="D190" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E190">
         <v>1</v>
@@ -14755,7 +14756,7 @@
         <v>302</v>
       </c>
       <c r="AB190" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC190" s="21"/>
       <c r="AD190" s="21"/>
@@ -14799,7 +14800,7 @@
         <v>22</v>
       </c>
       <c r="D191" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E191">
         <v>1</v>
@@ -14833,7 +14834,7 @@
         <v>640</v>
       </c>
       <c r="AB191" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC191" s="21"/>
       <c r="AD191" s="21"/>
@@ -14883,7 +14884,7 @@
         <v>22</v>
       </c>
       <c r="D192" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E192">
         <v>1</v>
@@ -14917,7 +14918,7 @@
         <v>640</v>
       </c>
       <c r="AB192" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC192" s="21"/>
       <c r="AD192" s="21"/>
@@ -14967,7 +14968,7 @@
         <v>22</v>
       </c>
       <c r="D193" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E193">
         <v>1</v>
@@ -15001,7 +15002,7 @@
         <v>640</v>
       </c>
       <c r="AB193" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC193" s="21"/>
       <c r="AD193" s="21"/>
@@ -15057,7 +15058,7 @@
         <v>22</v>
       </c>
       <c r="D194" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E194">
         <v>1</v>
@@ -15091,7 +15092,7 @@
         <v>640</v>
       </c>
       <c r="AB194" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC194" s="21"/>
       <c r="AD194" s="21"/>
@@ -15138,7 +15139,7 @@
     </row>
     <row r="195" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H195" s="23"/>
       <c r="I195" s="1"/>
@@ -15178,7 +15179,7 @@
         <v>701</v>
       </c>
       <c r="D196" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E196">
         <v>1</v>
@@ -15212,7 +15213,7 @@
         <v>614</v>
       </c>
       <c r="AB196" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC196" s="21"/>
       <c r="AD196" s="21"/>
@@ -15251,7 +15252,7 @@
         <v>701</v>
       </c>
       <c r="D197" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E197">
         <v>1</v>
@@ -15285,7 +15286,7 @@
         <v>614</v>
       </c>
       <c r="AB197" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC197" s="21"/>
       <c r="AD197" s="21"/>
@@ -15324,7 +15325,7 @@
         <v>701</v>
       </c>
       <c r="D198" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E198">
         <v>1</v>
@@ -15358,7 +15359,7 @@
         <v>614</v>
       </c>
       <c r="AB198" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC198" s="21"/>
       <c r="AD198" s="21"/>
@@ -15397,7 +15398,7 @@
         <v>701</v>
       </c>
       <c r="D199" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E199">
         <v>1</v>
@@ -15431,7 +15432,7 @@
         <v>614</v>
       </c>
       <c r="AB199" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC199" s="21"/>
       <c r="AD199" s="21"/>
@@ -15461,7 +15462,7 @@
     </row>
     <row r="200" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="H200" s="23"/>
       <c r="I200" s="1"/>
@@ -15492,7 +15493,7 @@
     </row>
     <row r="201" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E201">
         <v>1</v>
@@ -15504,7 +15505,7 @@
         <v>403</v>
       </c>
       <c r="D202" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E202">
         <v>1</v>
@@ -15522,7 +15523,7 @@
         <v>22</v>
       </c>
       <c r="D203" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E203">
         <v>1</v>
@@ -15554,7 +15555,7 @@
         <v>22</v>
       </c>
       <c r="D204" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E204">
         <v>1</v>
@@ -15586,7 +15587,7 @@
         <v>22</v>
       </c>
       <c r="D205" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E205">
         <v>1</v>
@@ -15633,7 +15634,7 @@
         <v>22</v>
       </c>
       <c r="D206" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E206">
         <v>1</v>
@@ -15683,7 +15684,7 @@
         <v>22</v>
       </c>
       <c r="D207" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E207">
         <v>1</v>
@@ -15733,7 +15734,7 @@
         <v>22</v>
       </c>
       <c r="D208" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E208">
         <v>1</v>
@@ -15762,7 +15763,7 @@
         <v>22</v>
       </c>
       <c r="D209" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E209">
         <v>1</v>
@@ -15794,7 +15795,7 @@
         <v>22</v>
       </c>
       <c r="D210" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E210">
         <v>1</v>
@@ -15844,7 +15845,7 @@
         <v>22</v>
       </c>
       <c r="D211" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E211">
         <v>1</v>
@@ -15894,7 +15895,7 @@
         <v>22</v>
       </c>
       <c r="D212" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E212">
         <v>1</v>
@@ -15944,7 +15945,7 @@
         <v>22</v>
       </c>
       <c r="D213" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E213">
         <v>1</v>
@@ -15994,7 +15995,7 @@
         <v>22</v>
       </c>
       <c r="D214" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E214">
         <v>1</v>
@@ -16035,7 +16036,7 @@
     </row>
     <row r="215" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
-        <v>771</v>
+        <v>23</v>
       </c>
       <c r="E215">
         <v>1</v>
@@ -16848,7 +16849,7 @@
         <v>431</v>
       </c>
       <c r="AB234" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC234" s="21"/>
       <c r="AD234" s="21"/>
@@ -16941,7 +16942,7 @@
         <v>87</v>
       </c>
       <c r="AB235" s="21" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AC235" s="21"/>
       <c r="AD235" s="21"/>
@@ -18644,7 +18645,7 @@
         <v>126</v>
       </c>
       <c r="G274" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H274" s="6" t="s">
         <v>24</v>
@@ -18668,7 +18669,7 @@
         <v>125</v>
       </c>
       <c r="AB274" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF274" s="5"/>
       <c r="AG274" s="5"/>
@@ -18694,7 +18695,7 @@
         <v>126</v>
       </c>
       <c r="G275" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H275" s="6" t="s">
         <v>24</v>
@@ -18718,7 +18719,7 @@
         <v>125</v>
       </c>
       <c r="AB275" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF275" s="5"/>
       <c r="AG275" s="5"/>
@@ -18744,7 +18745,7 @@
         <v>126</v>
       </c>
       <c r="G276" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H276" s="6" t="s">
         <v>24</v>
@@ -18768,7 +18769,7 @@
         <v>125</v>
       </c>
       <c r="AB276" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF276" s="5"/>
       <c r="AG276" s="5"/>
@@ -18794,7 +18795,7 @@
         <v>126</v>
       </c>
       <c r="G277" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H277" s="6" t="s">
         <v>24</v>
@@ -18818,7 +18819,7 @@
         <v>125</v>
       </c>
       <c r="AB277" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF277" s="5"/>
       <c r="AG277" s="5"/>
@@ -18844,7 +18845,7 @@
         <v>126</v>
       </c>
       <c r="G278" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H278" s="6" t="s">
         <v>24</v>
@@ -18868,7 +18869,7 @@
         <v>125</v>
       </c>
       <c r="AB278" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF278" s="5"/>
       <c r="AG278" s="5"/>
@@ -18894,7 +18895,7 @@
         <v>126</v>
       </c>
       <c r="G279" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H279" s="6" t="s">
         <v>24</v>
@@ -18918,7 +18919,7 @@
         <v>125</v>
       </c>
       <c r="AB279" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF279" s="5"/>
       <c r="AG279" s="5"/>
@@ -19598,7 +19599,7 @@
         <v>506</v>
       </c>
       <c r="G297" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H297" s="6" t="s">
         <v>24</v>
@@ -19622,7 +19623,7 @@
         <v>35</v>
       </c>
       <c r="AB297" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF297" s="5"/>
       <c r="AG297" s="5"/>
@@ -19651,7 +19652,7 @@
         <v>506</v>
       </c>
       <c r="G298" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H298" s="6" t="s">
         <v>24</v>
@@ -19675,7 +19676,7 @@
         <v>35</v>
       </c>
       <c r="AB298" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF298" s="5"/>
       <c r="AG298" s="5"/>
@@ -19704,7 +19705,7 @@
         <v>506</v>
       </c>
       <c r="G299" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H299" s="6" t="s">
         <v>24</v>
@@ -19728,7 +19729,7 @@
         <v>35</v>
       </c>
       <c r="AB299" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF299" s="5"/>
       <c r="AG299" s="5"/>
@@ -19757,7 +19758,7 @@
         <v>506</v>
       </c>
       <c r="G300" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H300" s="6" t="s">
         <v>24</v>
@@ -19781,7 +19782,7 @@
         <v>35</v>
       </c>
       <c r="AB300" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF300" s="5"/>
       <c r="AG300" s="5"/>
@@ -19810,7 +19811,7 @@
         <v>506</v>
       </c>
       <c r="G301" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H301" s="6" t="s">
         <v>24</v>
@@ -19834,7 +19835,7 @@
         <v>35</v>
       </c>
       <c r="AB301" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF301" s="5"/>
       <c r="AG301" s="5"/>
@@ -19863,7 +19864,7 @@
         <v>506</v>
       </c>
       <c r="G302" s="5" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="H302" s="6" t="s">
         <v>24</v>
@@ -19887,7 +19888,7 @@
         <v>35</v>
       </c>
       <c r="AB302" t="s">
-        <v>85</v>
+        <v>771</v>
       </c>
       <c r="AF302" s="5"/>
       <c r="AG302" s="5"/>
@@ -19897,246 +19898,246 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG67"/>
+  <autoFilter ref="A1:BG67" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B30:B31"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="H5" r:id="rId3"/>
-    <hyperlink ref="H6" r:id="rId4"/>
-    <hyperlink ref="H7" r:id="rId5"/>
-    <hyperlink ref="H8" r:id="rId6"/>
-    <hyperlink ref="H9" r:id="rId7"/>
-    <hyperlink ref="H10" r:id="rId8"/>
-    <hyperlink ref="H11" r:id="rId9"/>
-    <hyperlink ref="H12" r:id="rId10"/>
-    <hyperlink ref="H13" r:id="rId11"/>
-    <hyperlink ref="H14" r:id="rId12"/>
-    <hyperlink ref="H15" r:id="rId13"/>
-    <hyperlink ref="H16" r:id="rId14"/>
-    <hyperlink ref="H17" r:id="rId15"/>
-    <hyperlink ref="H18" r:id="rId16"/>
-    <hyperlink ref="H19" r:id="rId17"/>
-    <hyperlink ref="H20" r:id="rId18"/>
-    <hyperlink ref="H21" r:id="rId19"/>
-    <hyperlink ref="H22" r:id="rId20"/>
-    <hyperlink ref="H23" r:id="rId21"/>
-    <hyperlink ref="H24" r:id="rId22"/>
-    <hyperlink ref="H25" r:id="rId23"/>
-    <hyperlink ref="H27" r:id="rId24"/>
-    <hyperlink ref="H28" r:id="rId25"/>
-    <hyperlink ref="H29" r:id="rId26"/>
-    <hyperlink ref="H30" r:id="rId27"/>
-    <hyperlink ref="H31" r:id="rId28"/>
-    <hyperlink ref="H32" r:id="rId29"/>
-    <hyperlink ref="H33" r:id="rId30"/>
-    <hyperlink ref="H34" r:id="rId31"/>
-    <hyperlink ref="H35" r:id="rId32"/>
-    <hyperlink ref="H36" r:id="rId33"/>
-    <hyperlink ref="H37" r:id="rId34"/>
-    <hyperlink ref="H38" r:id="rId35"/>
-    <hyperlink ref="H39" r:id="rId36"/>
-    <hyperlink ref="H40" r:id="rId37"/>
-    <hyperlink ref="H41" r:id="rId38"/>
-    <hyperlink ref="H42" r:id="rId39"/>
-    <hyperlink ref="H43" r:id="rId40"/>
-    <hyperlink ref="H44" r:id="rId41"/>
-    <hyperlink ref="H45" r:id="rId42"/>
-    <hyperlink ref="H46" r:id="rId43"/>
-    <hyperlink ref="H47" r:id="rId44"/>
-    <hyperlink ref="H48" r:id="rId45"/>
-    <hyperlink ref="H49" r:id="rId46"/>
-    <hyperlink ref="H50" r:id="rId47"/>
-    <hyperlink ref="H51" r:id="rId48"/>
-    <hyperlink ref="H52" r:id="rId49"/>
-    <hyperlink ref="H53" r:id="rId50"/>
-    <hyperlink ref="H54" r:id="rId51"/>
-    <hyperlink ref="H56" r:id="rId52"/>
-    <hyperlink ref="H57" r:id="rId53"/>
-    <hyperlink ref="H55" r:id="rId54"/>
-    <hyperlink ref="H58" r:id="rId55"/>
-    <hyperlink ref="H59" r:id="rId56"/>
-    <hyperlink ref="H60" r:id="rId57"/>
-    <hyperlink ref="H61" r:id="rId58"/>
-    <hyperlink ref="H62" r:id="rId59"/>
-    <hyperlink ref="Z63" r:id="rId60"/>
-    <hyperlink ref="Z64" r:id="rId61"/>
-    <hyperlink ref="H63" r:id="rId62"/>
-    <hyperlink ref="H64" r:id="rId63"/>
-    <hyperlink ref="Z65" r:id="rId64"/>
-    <hyperlink ref="H65" r:id="rId65"/>
-    <hyperlink ref="Z66" r:id="rId66"/>
-    <hyperlink ref="H66" r:id="rId67"/>
-    <hyperlink ref="Z67" r:id="rId68"/>
-    <hyperlink ref="H67" r:id="rId69"/>
-    <hyperlink ref="H75" r:id="rId70"/>
-    <hyperlink ref="H76" r:id="rId71"/>
-    <hyperlink ref="H77" r:id="rId72"/>
-    <hyperlink ref="H78" r:id="rId73"/>
-    <hyperlink ref="H79" r:id="rId74"/>
-    <hyperlink ref="H80" r:id="rId75"/>
-    <hyperlink ref="H81" r:id="rId76"/>
-    <hyperlink ref="H82" r:id="rId77"/>
-    <hyperlink ref="H83" r:id="rId78"/>
-    <hyperlink ref="H84" r:id="rId79"/>
-    <hyperlink ref="H85" r:id="rId80"/>
-    <hyperlink ref="H86" r:id="rId81"/>
-    <hyperlink ref="H87" r:id="rId82"/>
-    <hyperlink ref="H88" r:id="rId83"/>
-    <hyperlink ref="H89" r:id="rId84"/>
-    <hyperlink ref="H90" r:id="rId85"/>
-    <hyperlink ref="H91" r:id="rId86"/>
-    <hyperlink ref="H100" r:id="rId87"/>
-    <hyperlink ref="H102" r:id="rId88"/>
-    <hyperlink ref="H101" r:id="rId89"/>
-    <hyperlink ref="H103" r:id="rId90"/>
-    <hyperlink ref="H104" r:id="rId91"/>
-    <hyperlink ref="H106" r:id="rId92"/>
-    <hyperlink ref="H105" r:id="rId93"/>
-    <hyperlink ref="H107" r:id="rId94"/>
-    <hyperlink ref="H108" r:id="rId95"/>
-    <hyperlink ref="H112" r:id="rId96"/>
-    <hyperlink ref="H111" r:id="rId97"/>
-    <hyperlink ref="H113" r:id="rId98"/>
-    <hyperlink ref="H114" r:id="rId99"/>
-    <hyperlink ref="H115" r:id="rId100"/>
-    <hyperlink ref="H116" r:id="rId101"/>
-    <hyperlink ref="H118" r:id="rId102"/>
-    <hyperlink ref="H119" r:id="rId103"/>
-    <hyperlink ref="H120" r:id="rId104"/>
-    <hyperlink ref="H121" r:id="rId105"/>
-    <hyperlink ref="H122" r:id="rId106"/>
-    <hyperlink ref="H123" r:id="rId107"/>
-    <hyperlink ref="H124" r:id="rId108"/>
-    <hyperlink ref="H126" r:id="rId109"/>
-    <hyperlink ref="H127" r:id="rId110"/>
-    <hyperlink ref="H128" r:id="rId111"/>
-    <hyperlink ref="H129" r:id="rId112"/>
-    <hyperlink ref="H130" r:id="rId113"/>
-    <hyperlink ref="H131" r:id="rId114"/>
-    <hyperlink ref="H132" r:id="rId115"/>
-    <hyperlink ref="H134" r:id="rId116"/>
-    <hyperlink ref="H135" r:id="rId117"/>
-    <hyperlink ref="H136" r:id="rId118"/>
-    <hyperlink ref="H137" r:id="rId119"/>
-    <hyperlink ref="H138" r:id="rId120"/>
-    <hyperlink ref="H139" r:id="rId121"/>
-    <hyperlink ref="H142" r:id="rId122"/>
-    <hyperlink ref="H143" r:id="rId123"/>
-    <hyperlink ref="H144" r:id="rId124"/>
-    <hyperlink ref="H145" r:id="rId125"/>
-    <hyperlink ref="H146" r:id="rId126"/>
-    <hyperlink ref="H147" r:id="rId127"/>
-    <hyperlink ref="H150" r:id="rId128"/>
-    <hyperlink ref="H151" r:id="rId129"/>
-    <hyperlink ref="H152" r:id="rId130"/>
-    <hyperlink ref="H153" r:id="rId131"/>
-    <hyperlink ref="H154" r:id="rId132"/>
-    <hyperlink ref="H155" r:id="rId133"/>
-    <hyperlink ref="H156" r:id="rId134"/>
-    <hyperlink ref="H158" r:id="rId135"/>
-    <hyperlink ref="H159" r:id="rId136"/>
-    <hyperlink ref="H160" r:id="rId137"/>
-    <hyperlink ref="H161" r:id="rId138"/>
-    <hyperlink ref="H162" r:id="rId139"/>
-    <hyperlink ref="H163" r:id="rId140"/>
-    <hyperlink ref="H234" r:id="rId141"/>
-    <hyperlink ref="H235" r:id="rId142"/>
-    <hyperlink ref="H166" r:id="rId143"/>
-    <hyperlink ref="H167" r:id="rId144"/>
-    <hyperlink ref="H168" r:id="rId145"/>
-    <hyperlink ref="H169" r:id="rId146"/>
-    <hyperlink ref="H170" r:id="rId147"/>
-    <hyperlink ref="H171" r:id="rId148"/>
-    <hyperlink ref="H233" r:id="rId149"/>
-    <hyperlink ref="H232" r:id="rId150"/>
-    <hyperlink ref="H231" r:id="rId151"/>
-    <hyperlink ref="H230" r:id="rId152"/>
-    <hyperlink ref="H182" r:id="rId153"/>
-    <hyperlink ref="H183" r:id="rId154"/>
-    <hyperlink ref="H184" r:id="rId155"/>
-    <hyperlink ref="H185" r:id="rId156"/>
-    <hyperlink ref="H186" r:id="rId157"/>
-    <hyperlink ref="H187" r:id="rId158"/>
-    <hyperlink ref="H174" r:id="rId159"/>
-    <hyperlink ref="H175" r:id="rId160"/>
-    <hyperlink ref="H176" r:id="rId161"/>
-    <hyperlink ref="H177" r:id="rId162"/>
-    <hyperlink ref="H178" r:id="rId163"/>
-    <hyperlink ref="H179" r:id="rId164"/>
-    <hyperlink ref="H26" r:id="rId165"/>
-    <hyperlink ref="H196" r:id="rId166"/>
-    <hyperlink ref="H189" r:id="rId167"/>
-    <hyperlink ref="H190" r:id="rId168"/>
-    <hyperlink ref="H191" r:id="rId169"/>
-    <hyperlink ref="H192" r:id="rId170"/>
-    <hyperlink ref="H193" r:id="rId171"/>
-    <hyperlink ref="H194" r:id="rId172"/>
-    <hyperlink ref="H197" r:id="rId173"/>
-    <hyperlink ref="H198" r:id="rId174"/>
-    <hyperlink ref="H199" r:id="rId175"/>
-    <hyperlink ref="Z238" r:id="rId176"/>
-    <hyperlink ref="H238" r:id="rId177"/>
-    <hyperlink ref="H69" r:id="rId178"/>
-    <hyperlink ref="H70" r:id="rId179"/>
-    <hyperlink ref="H71" r:id="rId180"/>
-    <hyperlink ref="H72" r:id="rId181"/>
-    <hyperlink ref="H73" r:id="rId182"/>
-    <hyperlink ref="H109" r:id="rId183"/>
-    <hyperlink ref="H94" r:id="rId184"/>
-    <hyperlink ref="H95" r:id="rId185"/>
-    <hyperlink ref="H96" r:id="rId186"/>
-    <hyperlink ref="H97" r:id="rId187"/>
-    <hyperlink ref="H249" r:id="rId188"/>
-    <hyperlink ref="H250" r:id="rId189"/>
-    <hyperlink ref="H251" r:id="rId190"/>
-    <hyperlink ref="H252" r:id="rId191"/>
-    <hyperlink ref="H253" r:id="rId192"/>
-    <hyperlink ref="H254" r:id="rId193"/>
-    <hyperlink ref="H255" r:id="rId194"/>
-    <hyperlink ref="H257" r:id="rId195"/>
-    <hyperlink ref="H258" r:id="rId196"/>
-    <hyperlink ref="H259" r:id="rId197"/>
-    <hyperlink ref="H260" r:id="rId198"/>
-    <hyperlink ref="H261" r:id="rId199"/>
-    <hyperlink ref="H262" r:id="rId200"/>
-    <hyperlink ref="H263" r:id="rId201"/>
-    <hyperlink ref="H266" r:id="rId202"/>
-    <hyperlink ref="H267" r:id="rId203"/>
-    <hyperlink ref="H268" r:id="rId204"/>
-    <hyperlink ref="H269" r:id="rId205"/>
-    <hyperlink ref="H270" r:id="rId206"/>
-    <hyperlink ref="H271" r:id="rId207"/>
-    <hyperlink ref="H272" r:id="rId208"/>
-    <hyperlink ref="H274" r:id="rId209"/>
-    <hyperlink ref="H275" r:id="rId210"/>
-    <hyperlink ref="H276" r:id="rId211"/>
-    <hyperlink ref="H277" r:id="rId212"/>
-    <hyperlink ref="H278" r:id="rId213"/>
-    <hyperlink ref="H279" r:id="rId214"/>
-    <hyperlink ref="H283" r:id="rId215"/>
-    <hyperlink ref="H284" r:id="rId216"/>
-    <hyperlink ref="H285" r:id="rId217"/>
-    <hyperlink ref="H286" r:id="rId218"/>
-    <hyperlink ref="H287" r:id="rId219"/>
-    <hyperlink ref="H288" r:id="rId220"/>
-    <hyperlink ref="H290" r:id="rId221"/>
-    <hyperlink ref="H291" r:id="rId222"/>
-    <hyperlink ref="H292" r:id="rId223"/>
-    <hyperlink ref="H293" r:id="rId224"/>
-    <hyperlink ref="H294" r:id="rId225"/>
-    <hyperlink ref="H295" r:id="rId226"/>
-    <hyperlink ref="H297" r:id="rId227"/>
-    <hyperlink ref="H298" r:id="rId228"/>
-    <hyperlink ref="H299" r:id="rId229"/>
-    <hyperlink ref="H300" r:id="rId230"/>
-    <hyperlink ref="H301" r:id="rId231"/>
-    <hyperlink ref="H302" r:id="rId232"/>
-    <hyperlink ref="H243" r:id="rId233"/>
-    <hyperlink ref="H244" r:id="rId234"/>
-    <hyperlink ref="H2" r:id="rId235"/>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="H16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="H19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="H21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="H23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="H24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="H25" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="H27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="H28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="H33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="H35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="H37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="H39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="H42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="H43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="H45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="H46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="H47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="H48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="H49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="H51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="H52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="H53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="H54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="H56" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="H57" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="H55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="H58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="H59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="H61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="H62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="Z63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="Z64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="H63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="H64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="Z65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="H65" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="Z66" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="H66" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="Z67" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="H67" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="H75" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="H76" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="H77" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="H78" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="H79" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="H80" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="H81" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="H82" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="H83" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="H84" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="H85" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="H86" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="H87" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="H88" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="H89" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="H90" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="H91" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="H100" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="H102" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="H101" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="H103" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="H104" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="H106" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="H105" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="H107" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="H108" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="H112" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="H111" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="H113" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="H114" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="H115" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="H116" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="H118" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="H119" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="H120" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="H121" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="H122" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="H123" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="H124" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="H126" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="H127" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="H128" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="H129" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="H130" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="H131" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="H132" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="H134" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="H135" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="H136" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="H137" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="H138" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="H139" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="H142" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="H143" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="H144" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="H145" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="H146" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="H147" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="H150" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="H151" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="H152" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="H153" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="H154" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="H155" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="H156" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="H158" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="H159" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="H160" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="H161" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="H162" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="H163" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="H234" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="H235" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="H166" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="H167" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="H168" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="H169" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="H170" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="H171" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="H233" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="H232" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="H231" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="H230" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="H182" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="H183" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="H184" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="H185" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="H186" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="H187" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="H174" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="H175" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="H176" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="H177" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="H178" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="H179" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="H26" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="H196" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="H189" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="H190" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="H191" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="H192" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="H193" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="H194" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="H197" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="H198" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="H199" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="Z238" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="H238" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="H69" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="H70" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="H71" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="H72" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="H73" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="H109" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="H94" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="H95" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="H96" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="H97" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="H249" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="H250" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="H251" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="H252" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="H253" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="H254" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="H255" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="H257" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="H258" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="H259" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="H260" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="H261" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="H262" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="H263" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="H266" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="H267" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="H268" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="H269" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="H270" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="H271" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="H272" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="H274" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="H275" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="H276" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="H277" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="H278" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="H279" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="H283" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="H284" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="H285" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="H286" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="H287" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="H288" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="H290" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="H291" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="H292" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="H293" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="H294" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="H295" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="H297" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="H298" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="H299" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="H300" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="H301" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="H302" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="H243" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="H244" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="H2" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId236"/>
@@ -20144,7 +20145,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AU92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27428,92 +27429,92 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26"/>
-    <hyperlink ref="I28" r:id="rId27"/>
-    <hyperlink ref="I29" r:id="rId28"/>
-    <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I32" r:id="rId31"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I34" r:id="rId33"/>
-    <hyperlink ref="I35" r:id="rId34"/>
-    <hyperlink ref="I36" r:id="rId35"/>
-    <hyperlink ref="I37" r:id="rId36"/>
-    <hyperlink ref="I38" r:id="rId37"/>
-    <hyperlink ref="I39" r:id="rId38"/>
-    <hyperlink ref="I40" r:id="rId39"/>
-    <hyperlink ref="I41" r:id="rId40"/>
-    <hyperlink ref="I42" r:id="rId41"/>
-    <hyperlink ref="I43" r:id="rId42"/>
-    <hyperlink ref="I44" r:id="rId43"/>
-    <hyperlink ref="I45" r:id="rId44"/>
-    <hyperlink ref="I46" r:id="rId45"/>
-    <hyperlink ref="I47" r:id="rId46"/>
-    <hyperlink ref="I48" r:id="rId47"/>
-    <hyperlink ref="I49" r:id="rId48"/>
-    <hyperlink ref="I50" r:id="rId49"/>
-    <hyperlink ref="I51" r:id="rId50"/>
-    <hyperlink ref="I52" r:id="rId51"/>
-    <hyperlink ref="I54" r:id="rId52"/>
-    <hyperlink ref="I55" r:id="rId53"/>
-    <hyperlink ref="I53" r:id="rId54"/>
-    <hyperlink ref="I56" r:id="rId55"/>
-    <hyperlink ref="I57" r:id="rId56"/>
-    <hyperlink ref="I58" r:id="rId57"/>
-    <hyperlink ref="I59" r:id="rId58"/>
-    <hyperlink ref="I60" r:id="rId59"/>
-    <hyperlink ref="Z61" r:id="rId60"/>
-    <hyperlink ref="Z62" r:id="rId61"/>
-    <hyperlink ref="I61" r:id="rId62"/>
-    <hyperlink ref="I62" r:id="rId63"/>
-    <hyperlink ref="Z63" r:id="rId64"/>
-    <hyperlink ref="I63" r:id="rId65"/>
-    <hyperlink ref="Z64" r:id="rId66"/>
-    <hyperlink ref="I64" r:id="rId67"/>
-    <hyperlink ref="Z65" r:id="rId68"/>
-    <hyperlink ref="I65" r:id="rId69"/>
-    <hyperlink ref="I66" r:id="rId70"/>
-    <hyperlink ref="I67" r:id="rId71"/>
-    <hyperlink ref="I68" r:id="rId72"/>
-    <hyperlink ref="I69" r:id="rId73"/>
-    <hyperlink ref="I70" r:id="rId74"/>
-    <hyperlink ref="I71" r:id="rId75"/>
-    <hyperlink ref="I72" r:id="rId76"/>
-    <hyperlink ref="I73" r:id="rId77"/>
-    <hyperlink ref="I74" r:id="rId78"/>
-    <hyperlink ref="I75" r:id="rId79"/>
-    <hyperlink ref="I76" r:id="rId80"/>
-    <hyperlink ref="I77" r:id="rId81"/>
-    <hyperlink ref="I78" r:id="rId82"/>
-    <hyperlink ref="I79" r:id="rId83"/>
-    <hyperlink ref="I80" r:id="rId84"/>
-    <hyperlink ref="I81" r:id="rId85"/>
-    <hyperlink ref="I82" r:id="rId86"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="I15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="I16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="I17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="I18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="I19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="I20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="I21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="I22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="I23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="I24" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="I25" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="I26" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="I27" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="I28" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="I29" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="I30" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="I31" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="I32" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="I33" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="I34" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="I35" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="I36" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="I37" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="I38" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="I39" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="I40" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="I41" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="I42" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="I43" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="I44" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="I45" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="I46" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="I47" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="I48" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="I49" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="I50" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="I51" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="I52" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="I54" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="I55" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="I53" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="I56" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="I57" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="I58" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="I59" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="I60" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="Z61" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="Z62" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="I61" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="I62" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="Z63" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="I63" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="Z64" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="I64" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="Z65" r:id="rId68" xr:uid="{00000000-0004-0000-0100-000043000000}"/>
+    <hyperlink ref="I65" r:id="rId69" xr:uid="{00000000-0004-0000-0100-000044000000}"/>
+    <hyperlink ref="I66" r:id="rId70" xr:uid="{00000000-0004-0000-0100-000045000000}"/>
+    <hyperlink ref="I67" r:id="rId71" xr:uid="{00000000-0004-0000-0100-000046000000}"/>
+    <hyperlink ref="I68" r:id="rId72" xr:uid="{00000000-0004-0000-0100-000047000000}"/>
+    <hyperlink ref="I69" r:id="rId73" xr:uid="{00000000-0004-0000-0100-000048000000}"/>
+    <hyperlink ref="I70" r:id="rId74" xr:uid="{00000000-0004-0000-0100-000049000000}"/>
+    <hyperlink ref="I71" r:id="rId75" xr:uid="{00000000-0004-0000-0100-00004A000000}"/>
+    <hyperlink ref="I72" r:id="rId76" xr:uid="{00000000-0004-0000-0100-00004B000000}"/>
+    <hyperlink ref="I73" r:id="rId77" xr:uid="{00000000-0004-0000-0100-00004C000000}"/>
+    <hyperlink ref="I74" r:id="rId78" xr:uid="{00000000-0004-0000-0100-00004D000000}"/>
+    <hyperlink ref="I75" r:id="rId79" xr:uid="{00000000-0004-0000-0100-00004E000000}"/>
+    <hyperlink ref="I76" r:id="rId80" xr:uid="{00000000-0004-0000-0100-00004F000000}"/>
+    <hyperlink ref="I77" r:id="rId81" xr:uid="{00000000-0004-0000-0100-000050000000}"/>
+    <hyperlink ref="I78" r:id="rId82" xr:uid="{00000000-0004-0000-0100-000051000000}"/>
+    <hyperlink ref="I79" r:id="rId83" xr:uid="{00000000-0004-0000-0100-000052000000}"/>
+    <hyperlink ref="I80" r:id="rId84" xr:uid="{00000000-0004-0000-0100-000053000000}"/>
+    <hyperlink ref="I81" r:id="rId85" xr:uid="{00000000-0004-0000-0100-000054000000}"/>
+    <hyperlink ref="I82" r:id="rId86" xr:uid="{00000000-0004-0000-0100-000055000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId87"/>
@@ -27521,7 +27522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AU92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34342,92 +34343,92 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="I3" r:id="rId2"/>
-    <hyperlink ref="I4" r:id="rId3"/>
-    <hyperlink ref="I5" r:id="rId4"/>
-    <hyperlink ref="I6" r:id="rId5"/>
-    <hyperlink ref="I7" r:id="rId6"/>
-    <hyperlink ref="I8" r:id="rId7"/>
-    <hyperlink ref="I9" r:id="rId8"/>
-    <hyperlink ref="I10" r:id="rId9"/>
-    <hyperlink ref="I11" r:id="rId10"/>
-    <hyperlink ref="I12" r:id="rId11"/>
-    <hyperlink ref="I13" r:id="rId12"/>
-    <hyperlink ref="I14" r:id="rId13"/>
-    <hyperlink ref="I15" r:id="rId14"/>
-    <hyperlink ref="I16" r:id="rId15"/>
-    <hyperlink ref="I17" r:id="rId16"/>
-    <hyperlink ref="I18" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
-    <hyperlink ref="I20" r:id="rId19"/>
-    <hyperlink ref="I21" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I23" r:id="rId22"/>
-    <hyperlink ref="I24" r:id="rId23"/>
-    <hyperlink ref="I25" r:id="rId24"/>
-    <hyperlink ref="I26" r:id="rId25"/>
-    <hyperlink ref="I27" r:id="rId26"/>
-    <hyperlink ref="I28" r:id="rId27"/>
-    <hyperlink ref="I29" r:id="rId28"/>
-    <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I32" r:id="rId31"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I34" r:id="rId33"/>
-    <hyperlink ref="I35" r:id="rId34"/>
-    <hyperlink ref="I36" r:id="rId35"/>
-    <hyperlink ref="I37" r:id="rId36"/>
-    <hyperlink ref="I38" r:id="rId37"/>
-    <hyperlink ref="I39" r:id="rId38"/>
-    <hyperlink ref="I40" r:id="rId39"/>
-    <hyperlink ref="I41" r:id="rId40"/>
-    <hyperlink ref="I42" r:id="rId41"/>
-    <hyperlink ref="I43" r:id="rId42"/>
-    <hyperlink ref="I44" r:id="rId43"/>
-    <hyperlink ref="I45" r:id="rId44"/>
-    <hyperlink ref="I46" r:id="rId45"/>
-    <hyperlink ref="I47" r:id="rId46"/>
-    <hyperlink ref="I48" r:id="rId47"/>
-    <hyperlink ref="I49" r:id="rId48"/>
-    <hyperlink ref="I50" r:id="rId49"/>
-    <hyperlink ref="I51" r:id="rId50"/>
-    <hyperlink ref="I52" r:id="rId51"/>
-    <hyperlink ref="I54" r:id="rId52"/>
-    <hyperlink ref="I55" r:id="rId53"/>
-    <hyperlink ref="I53" r:id="rId54"/>
-    <hyperlink ref="I56" r:id="rId55"/>
-    <hyperlink ref="I57" r:id="rId56"/>
-    <hyperlink ref="I58" r:id="rId57"/>
-    <hyperlink ref="I59" r:id="rId58"/>
-    <hyperlink ref="I60" r:id="rId59"/>
-    <hyperlink ref="Z61" r:id="rId60"/>
-    <hyperlink ref="Z62" r:id="rId61"/>
-    <hyperlink ref="I61" r:id="rId62"/>
-    <hyperlink ref="I62" r:id="rId63"/>
-    <hyperlink ref="Z63" r:id="rId64"/>
-    <hyperlink ref="I63" r:id="rId65"/>
-    <hyperlink ref="Z64" r:id="rId66"/>
-    <hyperlink ref="I64" r:id="rId67"/>
-    <hyperlink ref="Z65" r:id="rId68"/>
-    <hyperlink ref="I65" r:id="rId69"/>
-    <hyperlink ref="I66" r:id="rId70"/>
-    <hyperlink ref="I67" r:id="rId71"/>
-    <hyperlink ref="I68" r:id="rId72"/>
-    <hyperlink ref="I69" r:id="rId73"/>
-    <hyperlink ref="I70" r:id="rId74"/>
-    <hyperlink ref="I71" r:id="rId75"/>
-    <hyperlink ref="I72" r:id="rId76"/>
-    <hyperlink ref="I73" r:id="rId77"/>
-    <hyperlink ref="I74" r:id="rId78"/>
-    <hyperlink ref="I75" r:id="rId79"/>
-    <hyperlink ref="I76" r:id="rId80"/>
-    <hyperlink ref="I77" r:id="rId81"/>
-    <hyperlink ref="I78" r:id="rId82"/>
-    <hyperlink ref="I79" r:id="rId83"/>
-    <hyperlink ref="I80" r:id="rId84"/>
-    <hyperlink ref="I81" r:id="rId85"/>
-    <hyperlink ref="I82" r:id="rId86"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="I4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="I6" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="I7" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="I8" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="I9" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="I10" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="I11" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="I12" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="I13" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="I14" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="I15" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="I16" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="I17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="I18" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="I19" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="I20" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="I21" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="I22" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="I23" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="I24" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="I25" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="I26" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="I27" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="I28" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="I29" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="I30" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="I31" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="I32" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="I33" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="I34" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="I35" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="I36" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="I37" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="I38" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="I39" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="I40" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="I41" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="I42" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="I43" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="I44" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="I45" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="I46" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="I47" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="I48" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="I49" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="I50" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="I51" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="I52" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="I54" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="I55" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="I53" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="I56" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="I57" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="I58" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="I59" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="I60" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="Z61" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="Z62" r:id="rId61" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="I61" r:id="rId62" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="I62" r:id="rId63" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="Z63" r:id="rId64" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="I63" r:id="rId65" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="Z64" r:id="rId66" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="I64" r:id="rId67" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="Z65" r:id="rId68" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="I65" r:id="rId69" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="I66" r:id="rId70" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="I67" r:id="rId71" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="I68" r:id="rId72" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="I69" r:id="rId73" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="I70" r:id="rId74" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="I71" r:id="rId75" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="I72" r:id="rId76" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="I73" r:id="rId77" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="I74" r:id="rId78" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="I75" r:id="rId79" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="I76" r:id="rId80" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="I77" r:id="rId81" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
+    <hyperlink ref="I78" r:id="rId82" xr:uid="{00000000-0004-0000-0200-000051000000}"/>
+    <hyperlink ref="I79" r:id="rId83" xr:uid="{00000000-0004-0000-0200-000052000000}"/>
+    <hyperlink ref="I80" r:id="rId84" xr:uid="{00000000-0004-0000-0200-000053000000}"/>
+    <hyperlink ref="I81" r:id="rId85" xr:uid="{00000000-0004-0000-0200-000054000000}"/>
+    <hyperlink ref="I82" r:id="rId86" xr:uid="{00000000-0004-0000-0200-000055000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId87"/>
@@ -34435,7 +34436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Payment method for Amex ezeclick i updated
</commit_message>
<xml_diff>
--- a/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
+++ b/Airpay_Automation_Framework/AirPayTestData/TestData/Datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shishir.shah\AirpayAutomationProject_Updated\Airpay_Automation_Framework\AirPayTestData\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C435EA79-CBB0-421F-82C4-0215DBBD7777}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE64F00B-C138-407F-AD28-5FBE3CB6328B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="DataRequired" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NoramlKit!$A$1:$BG$228</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NoramlKit!$A$1:$BG$67</definedName>
   </definedNames>
   <calcPr calcId="152511" iterateDelta="1E-4"/>
   <extLst>
@@ -3122,14 +3122,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BY302"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O83" sqref="O83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3365,7 +3365,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="2" spans="1:59" s="4" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>766</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -3499,7 +3499,7 @@
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -3547,7 +3547,7 @@
         <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D5" t="s">
         <v>23</v>
@@ -3595,7 +3595,7 @@
         <v>339</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
@@ -3646,7 +3646,7 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D7" t="s">
         <v>23</v>
@@ -3683,7 +3683,7 @@
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
     </row>
-    <row r="8" spans="1:59" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:59" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>664</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:59" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:59" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>664</v>
       </c>
@@ -3769,7 +3769,7 @@
       <c r="AG9" s="5"/>
       <c r="AH9" s="5"/>
     </row>
-    <row r="10" spans="1:59" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:59" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>665</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
@@ -3882,7 +3882,7 @@
         <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D12" t="s">
         <v>23</v>
@@ -3942,7 +3942,7 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>
@@ -4002,7 +4002,7 @@
         <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D14" t="s">
         <v>23</v>
@@ -4047,7 +4047,7 @@
         <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D15" t="s">
         <v>23</v>
@@ -4107,7 +4107,7 @@
         <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D16" t="s">
         <v>23</v>
@@ -4167,7 +4167,7 @@
         <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D17" t="s">
         <v>23</v>
@@ -4227,7 +4227,7 @@
         <v>68</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
@@ -4287,7 +4287,7 @@
         <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
@@ -4339,7 +4339,7 @@
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
     </row>
-    <row r="20" spans="1:51" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:51" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>72</v>
       </c>
@@ -4397,7 +4397,7 @@
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
     </row>
-    <row r="21" spans="1:51" ht="17.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:51" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>74</v>
       </c>
@@ -4455,7 +4455,7 @@
       <c r="AG21" s="5"/>
       <c r="AH21" s="5"/>
     </row>
-    <row r="22" spans="1:51" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:51" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>75</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
     </row>
-    <row r="23" spans="1:51" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>673</v>
       </c>
@@ -4573,7 +4573,7 @@
       <c r="AG23" s="5"/>
       <c r="AH23" s="5"/>
     </row>
-    <row r="24" spans="1:51" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:51" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>674</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D25" t="s">
         <v>23</v>
@@ -4682,7 +4682,7 @@
         <v>628</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D26" t="s">
         <v>23</v>
@@ -4735,7 +4735,7 @@
         <v>84</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D27" t="s">
         <v>23</v>
@@ -4833,7 +4833,7 @@
         <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D29" t="s">
         <v>23</v>
@@ -4877,7 +4877,7 @@
         <v>770</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D30" t="s">
         <v>23</v>
@@ -4922,7 +4922,7 @@
       </c>
       <c r="B31" s="78"/>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D31" t="s">
         <v>23</v>
@@ -4966,7 +4966,7 @@
         <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D32" t="s">
         <v>23</v>
@@ -5013,7 +5013,7 @@
         <v>97</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D33" t="s">
         <v>23</v>
@@ -5060,7 +5060,7 @@
         <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D34" t="s">
         <v>23</v>
@@ -5107,7 +5107,7 @@
         <v>104</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D35" t="s">
         <v>23</v>
@@ -5156,7 +5156,7 @@
       </c>
       <c r="Y35" s="9"/>
     </row>
-    <row r="36" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>107</v>
       </c>
@@ -5211,7 +5211,7 @@
       </c>
       <c r="Y36" s="9"/>
     </row>
-    <row r="37" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="34" t="s">
         <v>108</v>
       </c>
@@ -5266,7 +5266,7 @@
       </c>
       <c r="Y37" s="9"/>
     </row>
-    <row r="38" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="34" t="s">
         <v>109</v>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="Y38" s="9"/>
     </row>
-    <row r="39" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
         <v>110</v>
       </c>
@@ -5376,7 +5376,7 @@
       </c>
       <c r="Y39" s="9"/>
     </row>
-    <row r="40" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="34" t="s">
         <v>110</v>
       </c>
@@ -5431,7 +5431,7 @@
       </c>
       <c r="Y40" s="9"/>
     </row>
-    <row r="41" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
         <v>111</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
         <v>112</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
         <v>113</v>
       </c>
@@ -5593,7 +5593,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="34" t="s">
         <v>114</v>
       </c>
@@ -5647,7 +5647,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="34" t="s">
         <v>115</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D46" t="s">
         <v>23</v>
@@ -5753,7 +5753,7 @@
         <v>631</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D47" t="s">
         <v>23</v>
@@ -5803,7 +5803,7 @@
         <v>135</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D48" t="s">
         <v>23</v>
@@ -5847,7 +5847,7 @@
         <v>136</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D49" t="s">
         <v>23</v>
@@ -5891,7 +5891,7 @@
         <v>134</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D50" t="s">
         <v>23</v>
@@ -5935,7 +5935,7 @@
         <v>138</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D51" t="s">
         <v>23</v>
@@ -5979,7 +5979,7 @@
         <v>140</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D52" t="s">
         <v>23</v>
@@ -6023,7 +6023,7 @@
         <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D53" t="s">
         <v>23</v>
@@ -6076,7 +6076,7 @@
         <v>155</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D54" t="s">
         <v>23</v>
@@ -6132,7 +6132,7 @@
         <v>159</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D55" t="s">
         <v>23</v>
@@ -6185,7 +6185,7 @@
         <v>156</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D56" t="s">
         <v>23</v>
@@ -6238,7 +6238,7 @@
         <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D57" t="s">
         <v>23</v>
@@ -6291,7 +6291,7 @@
         <v>161</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D58" t="s">
         <v>23</v>
@@ -6344,7 +6344,7 @@
         <v>165</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D59" t="s">
         <v>23</v>
@@ -6397,7 +6397,7 @@
         <v>166</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D60" t="s">
         <v>23</v>
@@ -6450,7 +6450,7 @@
         <v>167</v>
       </c>
       <c r="C61" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D61" t="s">
         <v>23</v>
@@ -6495,7 +6495,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="62" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="31" t="s">
         <v>173</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="34" t="s">
         <v>174</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="64" spans="1:34" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="34" t="s">
         <v>178</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="34" t="s">
         <v>180</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="34" t="s">
         <v>182</v>
       </c>
@@ -6705,7 +6705,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="34" t="s">
         <v>184</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="34"/>
       <c r="D68" t="s">
         <v>23</v>
@@ -6758,7 +6758,7 @@
       <c r="N68" s="9"/>
       <c r="Z68" s="16"/>
     </row>
-    <row r="69" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="34" t="s">
         <v>647</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="70" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="34" t="s">
         <v>648</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="71" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="34" t="s">
         <v>178</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="72" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="34" t="s">
         <v>655</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="34" t="s">
         <v>656</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="74" spans="1:57" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:57" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="34"/>
       <c r="C74" s="15"/>
       <c r="D74" t="s">
@@ -7088,7 +7088,7 @@
         <v>186</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D75" t="s">
         <v>23</v>
@@ -7132,7 +7132,7 @@
         <v>188</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D76" t="s">
         <v>23</v>
@@ -7185,7 +7185,7 @@
         <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D77" t="s">
         <v>23</v>
@@ -7238,7 +7238,7 @@
         <v>630</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D78" t="s">
         <v>23</v>
@@ -7287,7 +7287,7 @@
         <v>196</v>
       </c>
       <c r="C79" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D79" t="s">
         <v>23</v>
@@ -7331,7 +7331,7 @@
         <v>198</v>
       </c>
       <c r="C80" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D80" t="s">
         <v>23</v>
@@ -7372,7 +7372,7 @@
         <v>201</v>
       </c>
       <c r="C81" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D81" t="s">
         <v>23</v>
@@ -7413,7 +7413,7 @@
         <v>201</v>
       </c>
       <c r="C82" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D82" t="s">
         <v>23</v>
@@ -7454,7 +7454,7 @@
         <v>203</v>
       </c>
       <c r="C83" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D83" t="s">
         <v>23</v>
@@ -7495,7 +7495,7 @@
         <v>204</v>
       </c>
       <c r="C84" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D84" t="s">
         <v>23</v>
@@ -7536,7 +7536,7 @@
         <v>677</v>
       </c>
       <c r="C85" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D85" t="s">
         <v>23</v>
@@ -7582,7 +7582,7 @@
       <c r="AK85" s="17"/>
       <c r="AL85" s="17"/>
     </row>
-    <row r="86" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="34" t="s">
         <v>214</v>
       </c>
@@ -7636,7 +7636,7 @@
       <c r="AK86" s="17"/>
       <c r="AL86" s="17"/>
     </row>
-    <row r="87" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="34" t="s">
         <v>215</v>
       </c>
@@ -7690,7 +7690,7 @@
       <c r="AK87" s="17"/>
       <c r="AL87" s="17"/>
     </row>
-    <row r="88" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="34" t="s">
         <v>218</v>
       </c>
@@ -7744,7 +7744,7 @@
       <c r="AK88" s="17"/>
       <c r="AL88" s="17"/>
     </row>
-    <row r="89" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="34" t="s">
         <v>219</v>
       </c>
@@ -7798,7 +7798,7 @@
       <c r="AK89" s="17"/>
       <c r="AL89" s="17"/>
     </row>
-    <row r="90" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="34" t="s">
         <v>220</v>
       </c>
@@ -7852,7 +7852,7 @@
       <c r="AK90" s="17"/>
       <c r="AL90" s="17"/>
     </row>
-    <row r="91" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="34" t="s">
         <v>222</v>
       </c>
@@ -7906,7 +7906,7 @@
       <c r="AK91" s="17"/>
       <c r="AL91" s="17"/>
     </row>
-    <row r="92" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="34" t="s">
         <v>222</v>
       </c>
@@ -7929,13 +7929,13 @@
         <v>768</v>
       </c>
     </row>
-    <row r="93" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A93" s="34"/>
       <c r="D93" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="34" t="s">
         <v>683</v>
       </c>
@@ -7987,7 +7987,7 @@
       <c r="AK94" s="17"/>
       <c r="AL94" s="17"/>
     </row>
-    <row r="95" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="34" t="s">
         <v>684</v>
       </c>
@@ -8039,7 +8039,7 @@
       <c r="AK95" s="17"/>
       <c r="AL95" s="17"/>
     </row>
-    <row r="96" spans="1:38" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:38" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="34" t="s">
         <v>685</v>
       </c>
@@ -8091,7 +8091,7 @@
       <c r="AK96" s="17"/>
       <c r="AL96" s="17"/>
     </row>
-    <row r="97" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="34" t="s">
         <v>686</v>
       </c>
@@ -8135,13 +8135,13 @@
         <v>210</v>
       </c>
     </row>
-    <row r="98" spans="1:77" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A98" s="34"/>
       <c r="D98" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="34" t="s">
         <v>228</v>
       </c>
@@ -8179,7 +8179,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="34" t="s">
         <v>235</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="101" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="34" t="s">
         <v>238</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="102" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="34" t="s">
         <v>239</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="103" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="34" t="s">
         <v>240</v>
       </c>
@@ -8403,7 +8403,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="34" t="s">
         <v>241</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="34" t="s">
         <v>242</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="106" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="34" t="s">
         <v>243</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="107" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="34" t="s">
         <v>244</v>
       </c>
@@ -8627,7 +8627,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="108" spans="1:77" s="76" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:77" s="76" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="34" t="s">
         <v>245</v>
       </c>
@@ -8762,7 +8762,7 @@
       <c r="BX108" s="25"/>
       <c r="BY108" s="25"/>
     </row>
-    <row r="109" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="76" t="s">
         <v>247</v>
       </c>
@@ -8851,12 +8851,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="110" spans="1:77" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:77" x14ac:dyDescent="0.2">
       <c r="D110" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>265</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="112" spans="1:77" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:77" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>259</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="113" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>268</v>
       </c>
@@ -9108,7 +9108,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="114" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>267</v>
       </c>
@@ -9192,7 +9192,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="115" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>277</v>
       </c>
@@ -9282,7 +9282,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="116" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="117" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D117" t="s">
         <v>23</v>
       </c>
@@ -9401,7 +9401,7 @@
       <c r="AQ117" s="28"/>
       <c r="AR117" s="9"/>
     </row>
-    <row r="118" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>280</v>
       </c>
@@ -9482,7 +9482,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="119" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>284</v>
       </c>
@@ -9563,7 +9563,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="120" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>285</v>
       </c>
@@ -9644,7 +9644,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="121" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>286</v>
       </c>
@@ -9725,7 +9725,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="122" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>287</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="123" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>288</v>
       </c>
@@ -9905,7 +9905,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="124" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>290</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="125" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
         <v>23</v>
       </c>
@@ -10007,7 +10007,7 @@
       </c>
       <c r="I125" s="1"/>
     </row>
-    <row r="126" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>292</v>
       </c>
@@ -10091,7 +10091,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="127" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>297</v>
       </c>
@@ -10175,7 +10175,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="128" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>295</v>
       </c>
@@ -10259,7 +10259,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="129" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>296</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="130" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>298</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="131" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>299</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="132" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>300</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="133" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
         <v>23</v>
       </c>
@@ -10625,7 +10625,7 @@
       </c>
       <c r="I133" s="1"/>
     </row>
-    <row r="134" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>301</v>
       </c>
@@ -10712,7 +10712,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="135" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>304</v>
       </c>
@@ -10799,7 +10799,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="136" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>305</v>
       </c>
@@ -10883,7 +10883,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="137" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>306</v>
       </c>
@@ -10967,7 +10967,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="138" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>307</v>
       </c>
@@ -11057,7 +11057,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="139" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>308</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="140" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="29" t="s">
         <v>309</v>
       </c>
@@ -11159,7 +11159,7 @@
       </c>
       <c r="I140" s="1"/>
     </row>
-    <row r="141" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
         <v>23</v>
       </c>
@@ -11168,7 +11168,7 @@
       </c>
       <c r="I141" s="1"/>
     </row>
-    <row r="142" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>314</v>
       </c>
@@ -11255,7 +11255,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="143" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>315</v>
       </c>
@@ -11342,7 +11342,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="144" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>316</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="145" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>317</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="146" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>318</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="147" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>319</v>
       </c>
@@ -11690,7 +11690,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="148" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>23</v>
       </c>
@@ -11719,7 +11719,7 @@
       <c r="AQ148" s="28"/>
       <c r="AR148" s="9"/>
     </row>
-    <row r="149" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
         <v>23</v>
       </c>
@@ -11728,7 +11728,7 @@
       </c>
       <c r="I149" s="1"/>
     </row>
-    <row r="150" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>313</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="151" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>320</v>
       </c>
@@ -11902,7 +11902,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="152" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>321</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="153" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>322</v>
       </c>
@@ -12070,7 +12070,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="154" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>323</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="155" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>324</v>
       </c>
@@ -12250,7 +12250,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="156" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>327</v>
       </c>
@@ -12340,7 +12340,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="157" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
         <v>23</v>
       </c>
@@ -12349,7 +12349,7 @@
       </c>
       <c r="I157" s="1"/>
     </row>
-    <row r="158" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>330</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="159" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>331</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="160" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>332</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="161" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>333</v>
       </c>
@@ -12688,7 +12688,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="162" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>334</v>
       </c>
@@ -12778,7 +12778,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="163" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>335</v>
       </c>
@@ -12868,7 +12868,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="164" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
         <v>23</v>
       </c>
@@ -12899,7 +12899,7 @@
       <c r="AQ164" s="28"/>
       <c r="AR164" s="9"/>
     </row>
-    <row r="165" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
         <v>23</v>
       </c>
@@ -12930,7 +12930,7 @@
       <c r="AQ165" s="28"/>
       <c r="AR165" s="9"/>
     </row>
-    <row r="166" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>434</v>
       </c>
@@ -13014,7 +13014,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="167" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>435</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="168" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>436</v>
       </c>
@@ -13185,7 +13185,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="169" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>437</v>
       </c>
@@ -13269,7 +13269,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="170" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>438</v>
       </c>
@@ -13359,7 +13359,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="171" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>439</v>
       </c>
@@ -13449,7 +13449,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="172" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
         <v>23</v>
       </c>
@@ -13480,7 +13480,7 @@
       <c r="AQ172" s="28"/>
       <c r="AR172" s="9"/>
     </row>
-    <row r="173" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
         <v>23</v>
       </c>
@@ -13511,7 +13511,7 @@
       <c r="AQ173" s="28"/>
       <c r="AR173" s="9"/>
     </row>
-    <row r="174" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>452</v>
       </c>
@@ -13595,7 +13595,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="175" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>453</v>
       </c>
@@ -13682,7 +13682,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="176" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>454</v>
       </c>
@@ -13766,7 +13766,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="177" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>455</v>
       </c>
@@ -13850,7 +13850,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="178" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>456</v>
       </c>
@@ -13940,7 +13940,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="179" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>457</v>
       </c>
@@ -14030,7 +14030,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="180" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
         <v>23</v>
       </c>
@@ -14061,7 +14061,7 @@
       <c r="AQ180" s="28"/>
       <c r="AR180" s="9"/>
     </row>
-    <row r="181" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
         <v>23</v>
       </c>
@@ -14092,7 +14092,7 @@
       <c r="AQ181" s="28"/>
       <c r="AR181" s="9"/>
     </row>
-    <row r="182" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>442</v>
       </c>
@@ -14170,7 +14170,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="183" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>443</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="184" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>444</v>
       </c>
@@ -14335,7 +14335,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="185" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>445</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="186" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>446</v>
       </c>
@@ -14509,7 +14509,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="187" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>447</v>
       </c>
@@ -14599,7 +14599,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="188" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
         <v>23</v>
       </c>
@@ -14630,7 +14630,7 @@
       <c r="AQ188" s="28"/>
       <c r="AR188" s="9"/>
     </row>
-    <row r="189" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>633</v>
       </c>
@@ -14708,7 +14708,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="190" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>634</v>
       </c>
@@ -14789,7 +14789,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="191" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>635</v>
       </c>
@@ -14873,7 +14873,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="192" spans="1:44" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:44" ht="15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>636</v>
       </c>
@@ -14957,7 +14957,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="193" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>637</v>
       </c>
@@ -15047,7 +15047,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="194" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>638</v>
       </c>
@@ -15137,7 +15137,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="195" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
         <v>23</v>
       </c>
@@ -15176,7 +15176,7 @@
         <v>617</v>
       </c>
       <c r="C196" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D196" t="s">
         <v>23</v>
@@ -15249,7 +15249,7 @@
         <v>641</v>
       </c>
       <c r="C197" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D197" t="s">
         <v>23</v>
@@ -15322,7 +15322,7 @@
         <v>642</v>
       </c>
       <c r="C198" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D198" t="s">
         <v>23</v>
@@ -15395,7 +15395,7 @@
         <v>643</v>
       </c>
       <c r="C199" t="s">
-        <v>22</v>
+        <v>701</v>
       </c>
       <c r="D199" t="s">
         <v>23</v>
@@ -15460,7 +15460,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="200" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
         <v>23</v>
       </c>
@@ -15491,7 +15491,7 @@
       <c r="AQ200" s="28"/>
       <c r="AR200" s="9"/>
     </row>
-    <row r="201" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
         <v>23</v>
       </c>
@@ -15500,7 +15500,7 @@
       </c>
       <c r="I201" s="1"/>
     </row>
-    <row r="202" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>403</v>
       </c>
@@ -15512,7 +15512,7 @@
       </c>
       <c r="I202" s="1"/>
     </row>
-    <row r="203" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>397</v>
       </c>
@@ -15544,7 +15544,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="204" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>347</v>
       </c>
@@ -15576,7 +15576,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="205" spans="1:52" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="35" t="s">
         <v>354</v>
       </c>
@@ -15623,7 +15623,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="206" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>357</v>
       </c>
@@ -15673,7 +15673,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="207" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>358</v>
       </c>
@@ -15723,7 +15723,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="208" spans="1:52" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:52" ht="15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>361</v>
       </c>
@@ -15755,7 +15755,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="209" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>362</v>
       </c>
@@ -15784,7 +15784,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="210" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>366</v>
       </c>
@@ -15834,7 +15834,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="211" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>370</v>
       </c>
@@ -15884,7 +15884,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="212" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>377</v>
       </c>
@@ -15934,7 +15934,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="213" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>381</v>
       </c>
@@ -15984,7 +15984,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="214" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>385</v>
       </c>
@@ -16034,7 +16034,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="215" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
         <v>23</v>
       </c>
@@ -16043,7 +16043,7 @@
       </c>
       <c r="I215" s="1"/>
     </row>
-    <row r="216" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A216" s="20" t="s">
         <v>402</v>
       </c>
@@ -16052,7 +16052,7 @@
       </c>
       <c r="I216" s="1"/>
     </row>
-    <row r="217" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>391</v>
       </c>
@@ -16105,7 +16105,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="218" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>398</v>
       </c>
@@ -16138,7 +16138,7 @@
       </c>
       <c r="AM218" s="17"/>
     </row>
-    <row r="219" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>399</v>
       </c>
@@ -16170,7 +16170,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="220" spans="1:47" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="35" t="s">
         <v>400</v>
       </c>
@@ -16220,7 +16220,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="221" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>401</v>
       </c>
@@ -16267,7 +16267,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="222" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>404</v>
       </c>
@@ -16314,7 +16314,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="223" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>405</v>
       </c>
@@ -16346,7 +16346,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="224" spans="1:47" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:47" ht="15" x14ac:dyDescent="0.25">
       <c r="A224" s="36" t="s">
         <v>406</v>
       </c>
@@ -16396,7 +16396,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="225" spans="1:50" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A225" s="36" t="s">
         <v>411</v>
       </c>
@@ -16446,7 +16446,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="226" spans="1:50" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>414</v>
       </c>
@@ -16496,7 +16496,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="227" spans="1:50" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>417</v>
       </c>
@@ -16546,7 +16546,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="228" spans="1:50" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:50" ht="15" x14ac:dyDescent="0.25">
       <c r="E228">
         <v>1</v>
       </c>
@@ -19898,13 +19898,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BG228" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Y"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:BG67" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="B30:B31"/>
   </mergeCells>

</xml_diff>